<commit_message>
added new draft of fig 1
</commit_message>
<xml_diff>
--- a/rawdata/human/Iceland_fish_mammal_Harrison_31_07_24.xlsx
+++ b/rawdata/human/Iceland_fish_mammal_Harrison_31_07_24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gwm297/GitHubRepos/SC.Iceland/rawdata/human/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1E412F-E651-564A-9AF6-091E7A123A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FD26EB-AED8-AB4C-A24C-9F9BDBD606FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1880" yWindow="1880" windowWidth="34220" windowHeight="23880" activeTab="3" xr2:uid="{D189BD55-5742-4CB6-8B1D-37DCAD2EF093}"/>
+    <workbookView xWindow="10600" yWindow="500" windowWidth="34220" windowHeight="23880" activeTab="3" xr2:uid="{D189BD55-5742-4CB6-8B1D-37DCAD2EF093}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart_Harrison_010824" sheetId="3" r:id="rId1"/>
@@ -2327,7 +2327,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K38"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6189,7 +6189,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>